<commit_message>
docker push and deploy test
</commit_message>
<xml_diff>
--- a/app/games.xlsx
+++ b/app/games.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DevOps\Projects\Board-Game-Selector\Board-Game-Project\app\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DevOps\Projects\Board-Game-Selector\Main\app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46E336AD-161A-482E-A136-D9D3B14849AD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBFBF8AB-1968-4820-81AE-FE9ECD936A7D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6600" yWindow="5970" windowWidth="28800" windowHeight="15435" xr2:uid="{7195A62A-4848-4758-8152-4F74A79FE5C1}"/>
+    <workbookView xWindow="-28920" yWindow="1185" windowWidth="29040" windowHeight="15840" xr2:uid="{7195A62A-4848-4758-8152-4F74A79FE5C1}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>playersmin</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t>Tesla Vs Edison</t>
+  </si>
+  <si>
+    <t>Caverna</t>
   </si>
 </sst>
 </file>
@@ -421,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99730AD2-05BF-4B21-9823-57EF1894EEB4}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -498,7 +501,7 @@
         <v>2</v>
       </c>
       <c r="D4">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="E4" t="b">
         <v>1</v>
@@ -566,10 +569,27 @@
         <v>2</v>
       </c>
       <c r="D8">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="E8" t="b">
         <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>7</v>
+      </c>
+      <c r="D9">
+        <v>210</v>
+      </c>
+      <c r="E9" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>